<commit_message>
push changes gerardstlouis branch
</commit_message>
<xml_diff>
--- a/docs/Table Structure.xlsx
+++ b/docs/Table Structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ozimba\OneDrive\Onyx\KJAS_CarPark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\electron_apps\KJAS_CarPark\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{C32C0514-ECA3-4114-8F3F-114544E5D2C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{745FC3E5-28DA-4209-B777-93551ADBD83A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C95B31-EDE2-4B32-95C3-37B08492D435}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13830" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{88B9DFC2-BB34-44D6-ACC3-B2961EEBC608}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{88B9DFC2-BB34-44D6-ACC3-B2961EEBC608}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="35">
   <si>
     <t>User Table</t>
   </si>
@@ -496,24 +496,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF557BD-00FC-4EB1-BE2E-347A957A1A1D}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -521,7 +521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -529,7 +529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -537,7 +537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -545,7 +545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -553,7 +553,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -561,7 +561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -569,335 +569,343 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>24</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>33</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>3</v>
       </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>1</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>12</v>
       </c>
-      <c r="B28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>13</v>
       </c>
-      <c r="B29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>14</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>16</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>18</v>
       </c>
-      <c r="B32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>19</v>
       </c>
       <c r="B34" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>3</v>
       </c>
-      <c r="B35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>1</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>12</v>
       </c>
-      <c r="B40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>13</v>
       </c>
-      <c r="B41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>14</v>
-      </c>
-      <c r="B42" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>16</v>
       </c>
       <c r="B43" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>18</v>
       </c>
-      <c r="B44" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>19</v>
-      </c>
-      <c r="B45" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>26</v>
       </c>
       <c r="B46" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B48" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>30</v>
       </c>
-      <c r="B49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>31</v>
       </c>
-      <c r="B50" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>3</v>
       </c>
-      <c r="B51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="B52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>1</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>13</v>
       </c>
-      <c r="B56" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>34</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>18</v>
       </c>
-      <c r="B58" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="B59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>14</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>3</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>